<commit_message>
Adding timing files and timing reults to excel file. All data has been collected for algorithm 3.
</commit_message>
<xml_diff>
--- a/Project2Experiments.xlsx
+++ b/Project2Experiments.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t>A</t>
   </si>
@@ -48,6 +48,12 @@
   </si>
   <si>
     <t>V3(DP) (2000-2200)</t>
+  </si>
+  <si>
+    <t>DP Timing</t>
+  </si>
+  <si>
+    <t>Run time</t>
   </si>
 </sst>
 </file>
@@ -124,7 +130,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -137,6 +143,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -152,6 +159,1135 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Dynamic</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Programming Run Time vs Amount to Make Change </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$M$4:$M$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$N$4:$N$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>6.9999999999999999E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0000000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.9E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.1999999999999997E-5</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>1.07E-4</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>3.1300000000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>5.0699999999999996E-4</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>1.0759999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>2.5349999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>4.3930000000000002E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9C7E-4E43-9015-F06832D26D34}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="351873824"/>
+        <c:axId val="351874152"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="351873824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Amount</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> to make change (A)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="351874152"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="351874152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Run</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Time (s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="351873824"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -417,15 +1553,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:K256"/>
+  <dimension ref="C2:N256"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M65" sqref="M65"/>
+      <selection activeCell="M2" sqref="M2:N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
@@ -438,8 +1574,12 @@
         <v>4</v>
       </c>
       <c r="J2" s="3"/>
-    </row>
-    <row r="3" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N2" s="3"/>
+    </row>
+    <row r="3" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C3" s="6" t="s">
         <v>0</v>
       </c>
@@ -461,8 +1601,14 @@
         <v>1</v>
       </c>
       <c r="K3" s="7"/>
-    </row>
-    <row r="4" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C4" s="4">
         <v>1</v>
       </c>
@@ -483,8 +1629,14 @@
       <c r="J4" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M4" s="1">
+        <v>100</v>
+      </c>
+      <c r="N4" s="8">
+        <v>6.9999999999999999E-6</v>
+      </c>
+    </row>
+    <row r="5" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C5" s="4">
         <v>2</v>
       </c>
@@ -505,8 +1657,14 @@
       <c r="J5" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M5" s="1">
+        <v>200</v>
+      </c>
+      <c r="N5" s="8">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C6" s="4">
         <v>3</v>
       </c>
@@ -527,8 +1685,14 @@
       <c r="J6" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M6" s="1">
+        <v>500</v>
+      </c>
+      <c r="N6" s="8">
+        <v>2.9E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C7" s="4">
         <v>4</v>
       </c>
@@ -549,8 +1713,14 @@
       <c r="J7" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M7" s="1">
+        <v>1000</v>
+      </c>
+      <c r="N7" s="8">
+        <v>5.1999999999999997E-5</v>
+      </c>
+    </row>
+    <row r="8" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C8" s="4">
         <v>5</v>
       </c>
@@ -571,8 +1741,14 @@
       <c r="J8" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M8" s="1">
+        <v>2000</v>
+      </c>
+      <c r="N8" s="1">
+        <v>1.07E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C9" s="4">
         <v>6</v>
       </c>
@@ -593,8 +1769,14 @@
       <c r="J9" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M9" s="1">
+        <v>5000</v>
+      </c>
+      <c r="N9" s="1">
+        <v>3.1300000000000002E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C10" s="4">
         <v>7</v>
       </c>
@@ -615,8 +1797,14 @@
       <c r="J10" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M10" s="1">
+        <v>10000</v>
+      </c>
+      <c r="N10" s="1">
+        <v>5.0699999999999996E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C11" s="4">
         <v>8</v>
       </c>
@@ -637,8 +1825,14 @@
       <c r="J11" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M11" s="1">
+        <v>20000</v>
+      </c>
+      <c r="N11" s="1">
+        <v>1.0759999999999999E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C12" s="4">
         <v>9</v>
       </c>
@@ -659,8 +1853,14 @@
       <c r="J12" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M12" s="1">
+        <v>50000</v>
+      </c>
+      <c r="N12" s="1">
+        <v>2.5349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C13" s="4">
         <v>10</v>
       </c>
@@ -681,8 +1881,14 @@
       <c r="J13" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M13" s="1">
+        <v>100000</v>
+      </c>
+      <c r="N13" s="1">
+        <v>4.3930000000000002E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C14" s="4">
         <v>11</v>
       </c>
@@ -704,7 +1910,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C15" s="4">
         <v>12</v>
       </c>
@@ -726,7 +1932,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C16" s="4">
         <v>13</v>
       </c>
@@ -5599,5 +6805,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Algo 2 & micro timing
Updated the timing scheme to track microseconds
proj2timing.cpp now requires c++11 to compile use:

g++ -std=c++11 proj2timing.cpp -o timing

command to compile.
</commit_message>
<xml_diff>
--- a/Project2Experiments.xlsx
+++ b/Project2Experiments.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t>A</t>
   </si>
@@ -48,6 +48,12 @@
   </si>
   <si>
     <t>V3(DP) (2000-2200)</t>
+  </si>
+  <si>
+    <t>DP Timing</t>
+  </si>
+  <si>
+    <t>Run time</t>
   </si>
 </sst>
 </file>
@@ -124,7 +130,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -137,6 +143,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -152,6 +159,1135 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Dynamic</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Programming Run Time vs Amount to Make Change </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$M$4:$M$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$N$4:$N$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>6.9999999999999999E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0000000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.9E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.1999999999999997E-5</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>1.07E-4</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>3.1300000000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>5.0699999999999996E-4</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>1.0759999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>2.5349999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>4.3930000000000002E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9C7E-4E43-9015-F06832D26D34}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="351873824"/>
+        <c:axId val="351874152"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="351873824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Amount</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> to make change (A)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="351874152"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="351874152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Run</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Time (s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="351873824"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -417,15 +1553,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:K256"/>
+  <dimension ref="C2:N256"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M65" sqref="M65"/>
+      <selection activeCell="M2" sqref="M2:N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
@@ -438,8 +1574,12 @@
         <v>4</v>
       </c>
       <c r="J2" s="3"/>
-    </row>
-    <row r="3" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N2" s="3"/>
+    </row>
+    <row r="3" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C3" s="6" t="s">
         <v>0</v>
       </c>
@@ -461,8 +1601,14 @@
         <v>1</v>
       </c>
       <c r="K3" s="7"/>
-    </row>
-    <row r="4" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C4" s="4">
         <v>1</v>
       </c>
@@ -483,8 +1629,14 @@
       <c r="J4" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M4" s="1">
+        <v>100</v>
+      </c>
+      <c r="N4" s="8">
+        <v>6.9999999999999999E-6</v>
+      </c>
+    </row>
+    <row r="5" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C5" s="4">
         <v>2</v>
       </c>
@@ -505,8 +1657,14 @@
       <c r="J5" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M5" s="1">
+        <v>200</v>
+      </c>
+      <c r="N5" s="8">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C6" s="4">
         <v>3</v>
       </c>
@@ -527,8 +1685,14 @@
       <c r="J6" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M6" s="1">
+        <v>500</v>
+      </c>
+      <c r="N6" s="8">
+        <v>2.9E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C7" s="4">
         <v>4</v>
       </c>
@@ -549,8 +1713,14 @@
       <c r="J7" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M7" s="1">
+        <v>1000</v>
+      </c>
+      <c r="N7" s="8">
+        <v>5.1999999999999997E-5</v>
+      </c>
+    </row>
+    <row r="8" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C8" s="4">
         <v>5</v>
       </c>
@@ -571,8 +1741,14 @@
       <c r="J8" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M8" s="1">
+        <v>2000</v>
+      </c>
+      <c r="N8" s="1">
+        <v>1.07E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C9" s="4">
         <v>6</v>
       </c>
@@ -593,8 +1769,14 @@
       <c r="J9" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M9" s="1">
+        <v>5000</v>
+      </c>
+      <c r="N9" s="1">
+        <v>3.1300000000000002E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C10" s="4">
         <v>7</v>
       </c>
@@ -615,8 +1797,14 @@
       <c r="J10" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M10" s="1">
+        <v>10000</v>
+      </c>
+      <c r="N10" s="1">
+        <v>5.0699999999999996E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C11" s="4">
         <v>8</v>
       </c>
@@ -637,8 +1825,14 @@
       <c r="J11" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M11" s="1">
+        <v>20000</v>
+      </c>
+      <c r="N11" s="1">
+        <v>1.0759999999999999E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C12" s="4">
         <v>9</v>
       </c>
@@ -659,8 +1853,14 @@
       <c r="J12" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M12" s="1">
+        <v>50000</v>
+      </c>
+      <c r="N12" s="1">
+        <v>2.5349999999999999E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C13" s="4">
         <v>10</v>
       </c>
@@ -681,8 +1881,14 @@
       <c r="J13" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M13" s="1">
+        <v>100000</v>
+      </c>
+      <c r="N13" s="1">
+        <v>4.3930000000000002E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C14" s="4">
         <v>11</v>
       </c>
@@ -704,7 +1910,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C15" s="4">
         <v>12</v>
       </c>
@@ -726,7 +1932,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C16" s="4">
         <v>13</v>
       </c>
@@ -5599,5 +6805,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>